<commit_message>
Updated code for pre clinical trial
</commit_message>
<xml_diff>
--- a/Project_Details.xlsx
+++ b/Project_Details.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\NEU\Semester 1\AED\Aed Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\NEU\Java_Netbeans\Git_Final_Project\explorers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,15 +385,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -418,6 +409,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -824,16 +824,16 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="51.75" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -867,246 +867,276 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="102.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="19.5">
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6">
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>-1</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>-1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>-1</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>-1</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="7" t="s">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="B16" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A18" s="8" t="s">
+    <row r="17" spans="2:3" ht="15.75" thickBot="1"/>
+    <row r="18" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="68.25" thickBot="1">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="2:3" ht="68.25" thickBot="1">
+      <c r="B19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B20" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="68.25" thickBot="1">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="2:3" ht="68.25" thickBot="1">
+      <c r="B21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="45.75" thickBot="1">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="2:3" ht="45.75" thickBot="1">
+      <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="C23" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="23.25" thickBot="1">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="2:3" ht="23.25" thickBot="1">
+      <c r="B24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="C24" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B25" s="9" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>